<commit_message>
Adapt Class Generics. TODO: Kotlin preferred default values.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtJustConstructorSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtJustConstructorSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1ACDAB-1678-B34D-9E5A-53A3716389CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39489EB-3111-1044-A7B2-56ACD1879EDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>クラス名</t>
   </si>
@@ -410,6 +410,21 @@
   </si>
   <si>
     <t>BlancoValueObjectKtJustConstructorSample</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>typeNotSpecified</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>UnknownClass</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>未定義のクラス</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ミテイギノ </t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -507,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1018,12 +1033,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1210,6 +1245,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1621,10 +1668,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2418,21 +2465,48 @@
       <c r="O43" s="15"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="79"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="28"/>
+      <c r="A44" s="96">
+        <v>6</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="97"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="99"/>
+      <c r="J44" s="99"/>
+      <c r="K44" s="97" t="s">
+        <v>73</v>
+      </c>
+      <c r="L44" s="100"/>
+      <c r="M44" s="100"/>
+      <c r="N44" s="101"/>
       <c r="O44" s="15"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="24"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2451,7 +2525,7 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F60:J60" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:J61" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2464,7 +2538,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 G39:G44" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 G39:G45" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -2486,7 +2560,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H39:J44</xm:sqref>
+          <xm:sqref>H39:J45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>